<commit_message>
added Union - Right to Skate data
</commit_message>
<xml_diff>
--- a/koston/data/koston.xlsx
+++ b/koston/data/koston.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jared.wilber\Desktop\jenkem_data\koston\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3541180A-F2DD-4B8C-97AF-85B9C89E717B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91AF2448-E71A-453A-BC2A-DA7AF9D844DB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5644D466-66B3-4E17-B94A-2921DC353073}"/>
+    <workbookView xWindow="2240" yWindow="1800" windowWidth="14400" windowHeight="7360" xr2:uid="{5644D466-66B3-4E17-B94A-2921DC353073}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="87">
   <si>
     <t>clip_index</t>
   </si>
@@ -205,6 +205,93 @@
   </si>
   <si>
     <t>101 - WWII Report</t>
+  </si>
+  <si>
+    <t>backside flip</t>
+  </si>
+  <si>
+    <t>Union - Right to Skate</t>
+  </si>
+  <si>
+    <t>switch varial</t>
+  </si>
+  <si>
+    <t>fs 5-0 to switch crook</t>
+  </si>
+  <si>
+    <t>switch hardflip</t>
+  </si>
+  <si>
+    <t>switch bs noseslide 270</t>
+  </si>
+  <si>
+    <t>halfcab to noseslide to nosegrind to regular</t>
+  </si>
+  <si>
+    <t>nollie bs flip</t>
+  </si>
+  <si>
+    <t>bs tailslide</t>
+  </si>
+  <si>
+    <t>fs 180 nosegrind to noseslide to fakie</t>
+  </si>
+  <si>
+    <t>nollie noseslide to fakie</t>
+  </si>
+  <si>
+    <t>switch fs tailslide</t>
+  </si>
+  <si>
+    <t>nollie bs 180 to fakie 5-0</t>
+  </si>
+  <si>
+    <t>fs 5-0 to fs noseslide</t>
+  </si>
+  <si>
+    <t>switch bs noseslide 270 popover</t>
+  </si>
+  <si>
+    <t>switch bs flip</t>
+  </si>
+  <si>
+    <t>flatgap</t>
+  </si>
+  <si>
+    <t>switch big flip</t>
+  </si>
+  <si>
+    <t>bs tailslide to fakie</t>
+  </si>
+  <si>
+    <t>shootout</t>
+  </si>
+  <si>
+    <t>bs tailslide to fakie 5-0 to fakie</t>
+  </si>
+  <si>
+    <t>nollie fs tailslide</t>
+  </si>
+  <si>
+    <t>kickflip bs nosedlide to fakie</t>
+  </si>
+  <si>
+    <t>fs flip to switch manual to regular</t>
+  </si>
+  <si>
+    <t>melon grab</t>
+  </si>
+  <si>
+    <t>nollie fs 180</t>
+  </si>
+  <si>
+    <t>bs darkslide</t>
+  </si>
+  <si>
+    <t>halfcab heelflip to noseslide to fakie</t>
+  </si>
+  <si>
+    <t>switch flip bs tail</t>
   </si>
 </sst>
 </file>
@@ -556,11 +643,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA88418-AAB9-4F27-A456-87056BC11CAB}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J30" sqref="J30"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1272,6 +1359,651 @@
         <v>57</v>
       </c>
     </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
+        <v>24</v>
+      </c>
+      <c r="H35" t="s">
+        <v>52</v>
+      </c>
+      <c r="J35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>60</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="G36" t="s">
+        <v>24</v>
+      </c>
+      <c r="H36" t="s">
+        <v>52</v>
+      </c>
+      <c r="J36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37" t="s">
+        <v>61</v>
+      </c>
+      <c r="G37" t="s">
+        <v>14</v>
+      </c>
+      <c r="H37" t="s">
+        <v>52</v>
+      </c>
+      <c r="J37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>3</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="G38" t="s">
+        <v>24</v>
+      </c>
+      <c r="H38" t="s">
+        <v>52</v>
+      </c>
+      <c r="J38" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="G39" t="s">
+        <v>24</v>
+      </c>
+      <c r="H39" t="s">
+        <v>52</v>
+      </c>
+      <c r="J39" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="G40" t="s">
+        <v>14</v>
+      </c>
+      <c r="H40" t="s">
+        <v>52</v>
+      </c>
+      <c r="J40" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
+        <v>64</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="G41" t="s">
+        <v>14</v>
+      </c>
+      <c r="H41" t="s">
+        <v>52</v>
+      </c>
+      <c r="J41" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>5</v>
+      </c>
+      <c r="B42">
+        <v>8</v>
+      </c>
+      <c r="C42" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="G42" t="s">
+        <v>24</v>
+      </c>
+      <c r="J42" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>6</v>
+      </c>
+      <c r="B43">
+        <v>9</v>
+      </c>
+      <c r="C43" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="G43" t="s">
+        <v>14</v>
+      </c>
+      <c r="H43" t="s">
+        <v>52</v>
+      </c>
+      <c r="J43" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>6</v>
+      </c>
+      <c r="B44">
+        <v>10</v>
+      </c>
+      <c r="C44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="G44" t="s">
+        <v>14</v>
+      </c>
+      <c r="H44" t="s">
+        <v>52</v>
+      </c>
+      <c r="J44" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>6</v>
+      </c>
+      <c r="B45">
+        <v>11</v>
+      </c>
+      <c r="C45" t="s">
+        <v>29</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="G45" t="s">
+        <v>24</v>
+      </c>
+      <c r="J45" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>7</v>
+      </c>
+      <c r="B46">
+        <v>12</v>
+      </c>
+      <c r="C46" t="s">
+        <v>68</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="G46" t="s">
+        <v>14</v>
+      </c>
+      <c r="J46" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>7</v>
+      </c>
+      <c r="B47">
+        <v>13</v>
+      </c>
+      <c r="C47" t="s">
+        <v>69</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="G47" t="s">
+        <v>14</v>
+      </c>
+      <c r="J47" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>8</v>
+      </c>
+      <c r="B48">
+        <v>14</v>
+      </c>
+      <c r="C48" t="s">
+        <v>70</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="G48" t="s">
+        <v>14</v>
+      </c>
+      <c r="H48" t="s">
+        <v>52</v>
+      </c>
+      <c r="J48" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>9</v>
+      </c>
+      <c r="B49">
+        <v>15</v>
+      </c>
+      <c r="C49" t="s">
+        <v>71</v>
+      </c>
+      <c r="G49" t="s">
+        <v>14</v>
+      </c>
+      <c r="J49" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>10</v>
+      </c>
+      <c r="B50">
+        <v>16</v>
+      </c>
+      <c r="C50" t="s">
+        <v>72</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50" t="s">
+        <v>14</v>
+      </c>
+      <c r="H50" t="s">
+        <v>52</v>
+      </c>
+      <c r="J50" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>11</v>
+      </c>
+      <c r="B51">
+        <v>17</v>
+      </c>
+      <c r="C51" t="s">
+        <v>73</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="G51" t="s">
+        <v>24</v>
+      </c>
+      <c r="H51" t="s">
+        <v>74</v>
+      </c>
+      <c r="J51" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>12</v>
+      </c>
+      <c r="B52">
+        <v>18</v>
+      </c>
+      <c r="C52" t="s">
+        <v>75</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="G52" t="s">
+        <v>11</v>
+      </c>
+      <c r="J52" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>13</v>
+      </c>
+      <c r="B53">
+        <v>19</v>
+      </c>
+      <c r="C53" t="s">
+        <v>76</v>
+      </c>
+      <c r="G53" t="s">
+        <v>14</v>
+      </c>
+      <c r="H53" t="s">
+        <v>77</v>
+      </c>
+      <c r="J53" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>14</v>
+      </c>
+      <c r="B54">
+        <v>20</v>
+      </c>
+      <c r="C54" t="s">
+        <v>15</v>
+      </c>
+      <c r="G54" t="s">
+        <v>14</v>
+      </c>
+      <c r="H54" t="s">
+        <v>77</v>
+      </c>
+      <c r="J54" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>15</v>
+      </c>
+      <c r="B55">
+        <v>21</v>
+      </c>
+      <c r="C55" t="s">
+        <v>78</v>
+      </c>
+      <c r="G55" t="s">
+        <v>14</v>
+      </c>
+      <c r="H55" t="s">
+        <v>52</v>
+      </c>
+      <c r="J55" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>16</v>
+      </c>
+      <c r="B56">
+        <v>22</v>
+      </c>
+      <c r="C56" t="s">
+        <v>79</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="G56" t="s">
+        <v>14</v>
+      </c>
+      <c r="J56" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>17</v>
+      </c>
+      <c r="B57">
+        <v>23</v>
+      </c>
+      <c r="C57" t="s">
+        <v>80</v>
+      </c>
+      <c r="G57" t="s">
+        <v>14</v>
+      </c>
+      <c r="J57" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>18</v>
+      </c>
+      <c r="B58">
+        <v>24</v>
+      </c>
+      <c r="C58" t="s">
+        <v>81</v>
+      </c>
+      <c r="G58" t="s">
+        <v>17</v>
+      </c>
+      <c r="J58" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>19</v>
+      </c>
+      <c r="B59">
+        <v>25</v>
+      </c>
+      <c r="C59" t="s">
+        <v>82</v>
+      </c>
+      <c r="G59" t="s">
+        <v>34</v>
+      </c>
+      <c r="J59" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>20</v>
+      </c>
+      <c r="B60">
+        <v>26</v>
+      </c>
+      <c r="C60" t="s">
+        <v>83</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="G60" t="s">
+        <v>34</v>
+      </c>
+      <c r="I60" t="s">
+        <v>39</v>
+      </c>
+      <c r="J60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>21</v>
+      </c>
+      <c r="B61">
+        <v>27</v>
+      </c>
+      <c r="C61" t="s">
+        <v>84</v>
+      </c>
+      <c r="G61" t="s">
+        <v>14</v>
+      </c>
+      <c r="J61" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>22</v>
+      </c>
+      <c r="B62">
+        <v>28</v>
+      </c>
+      <c r="C62" t="s">
+        <v>76</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="G62" t="s">
+        <v>14</v>
+      </c>
+      <c r="J62" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>23</v>
+      </c>
+      <c r="B63">
+        <v>29</v>
+      </c>
+      <c r="C63" t="s">
+        <v>85</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="G63" t="s">
+        <v>14</v>
+      </c>
+      <c r="J63" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>24</v>
+      </c>
+      <c r="B64">
+        <v>30</v>
+      </c>
+      <c r="C64" t="s">
+        <v>86</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="G64" t="s">
+        <v>14</v>
+      </c>
+      <c r="H64" t="s">
+        <v>52</v>
+      </c>
+      <c r="J64" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added fully flared and nike vid
</commit_message>
<xml_diff>
--- a/koston/data/koston.xlsx
+++ b/koston/data/koston.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jared.wilber\Desktop\jenkem_data\koston\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6490ACC-CD6F-4960-8778-F8DEE25118B1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8412666B-668B-4030-8838-446CB189E1CE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5644D466-66B3-4E17-B94A-2921DC353073}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1321" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1754" uniqueCount="424">
   <si>
     <t>clip_index</t>
   </si>
@@ -1027,6 +1027,282 @@
   </si>
   <si>
     <t>switch flip to fs crook</t>
+  </si>
+  <si>
+    <t>Chocolate - The Chocolate Tour</t>
+  </si>
+  <si>
+    <t>fakie fs 5-0 to regular</t>
+  </si>
+  <si>
+    <t>switch bs 180 to 5-0</t>
+  </si>
+  <si>
+    <t>bs tailslide to bs shuv-it</t>
+  </si>
+  <si>
+    <t>kickflip to bs 5-0</t>
+  </si>
+  <si>
+    <t>switch varial heelflip</t>
+  </si>
+  <si>
+    <t>kickflip bs tailslide to fakie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kickflip to bs nosegrind  </t>
+  </si>
+  <si>
+    <t>fakie fs 5-0 to fakie fs flip</t>
+  </si>
+  <si>
+    <t>switch bs shuv-it to nosegrind to fakie fs shuv-it</t>
+  </si>
+  <si>
+    <t>bs noseblunt</t>
+  </si>
+  <si>
+    <t>taildrop to fs 5050</t>
+  </si>
+  <si>
+    <t>bs crailslide</t>
+  </si>
+  <si>
+    <t>over handrail</t>
+  </si>
+  <si>
+    <t>roof</t>
+  </si>
+  <si>
+    <t>fs noseblunt to nosemanual</t>
+  </si>
+  <si>
+    <t>ledge, manual</t>
+  </si>
+  <si>
+    <t>fakie 360 flip to switch manual</t>
+  </si>
+  <si>
+    <t>fs 180 to switch 5050</t>
+  </si>
+  <si>
+    <t>fakie fs crook</t>
+  </si>
+  <si>
+    <t>nollie bs bluntslide</t>
+  </si>
+  <si>
+    <t>nollie bs 360 heelflip</t>
+  </si>
+  <si>
+    <t>nollie fs crook</t>
+  </si>
+  <si>
+    <t>fakie fs crook to bs 5-0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fakie 360 flip </t>
+  </si>
+  <si>
+    <t>fakie switch fs bluntslide</t>
+  </si>
+  <si>
+    <t>switch fs shuv-it to nosegrind to revert</t>
+  </si>
+  <si>
+    <t>flatbar</t>
+  </si>
+  <si>
+    <t>fakie bs hurricant to 270</t>
+  </si>
+  <si>
+    <t>nollie inward heelflip to fs noseslide</t>
+  </si>
+  <si>
+    <t>fakie 5-0 to halfcab flip</t>
+  </si>
+  <si>
+    <t>heelflip nosemanual to bs nosegrind popout</t>
+  </si>
+  <si>
+    <t>manual, ledge</t>
+  </si>
+  <si>
+    <t>switch crook to manual to fs shuv-it</t>
+  </si>
+  <si>
+    <t>fakie fs flip to manual to 180 to switch manual</t>
+  </si>
+  <si>
+    <t>nollie fs bigspin to switch manual to switch bs bigspin</t>
+  </si>
+  <si>
+    <t>nollie bs 180 to switch manual to switch fs bigspin</t>
+  </si>
+  <si>
+    <t>bs flip to fakie manual to halfcab flip</t>
+  </si>
+  <si>
+    <t>kickflip to fs tailslide to fakie</t>
+  </si>
+  <si>
+    <t>bs lipslide to fs bluntslide</t>
+  </si>
+  <si>
+    <t>fakie fs heelflip</t>
+  </si>
+  <si>
+    <t>bs bigspin</t>
+  </si>
+  <si>
+    <t>gap to bank</t>
+  </si>
+  <si>
+    <t>switch bs heelflip</t>
+  </si>
+  <si>
+    <t>triple set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stair </t>
+  </si>
+  <si>
+    <t>fs tailslide to switch bs tailslide</t>
+  </si>
+  <si>
+    <t>double set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">switch bs bigspin  </t>
+  </si>
+  <si>
+    <t>switch fs shuv-it to switch bluntslide</t>
+  </si>
+  <si>
+    <t>nollie bs 180 to switch feeble to regular</t>
+  </si>
+  <si>
+    <t>fakie 360 flip</t>
+  </si>
+  <si>
+    <t>macba</t>
+  </si>
+  <si>
+    <t>Lakai - Fully Flared</t>
+  </si>
+  <si>
+    <t>Nike - The SB Chronicles Vol. 3</t>
+  </si>
+  <si>
+    <t>bs wallie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kickflip to manual </t>
+  </si>
+  <si>
+    <t>wallie</t>
+  </si>
+  <si>
+    <t>treestump</t>
+  </si>
+  <si>
+    <t>wall</t>
+  </si>
+  <si>
+    <t>fs bluntslide to 5050</t>
+  </si>
+  <si>
+    <t>pole jam</t>
+  </si>
+  <si>
+    <t>pole</t>
+  </si>
+  <si>
+    <t>bs boardslide pop-out</t>
+  </si>
+  <si>
+    <t>wallie to bs 5050</t>
+  </si>
+  <si>
+    <t>wall to ledge</t>
+  </si>
+  <si>
+    <t>pole jam to bs wallride</t>
+  </si>
+  <si>
+    <t>wall, over obstacle</t>
+  </si>
+  <si>
+    <t>bs bluntslide to fs 270</t>
+  </si>
+  <si>
+    <t>ledge to wall</t>
+  </si>
+  <si>
+    <t>bank to table</t>
+  </si>
+  <si>
+    <t>wallie to fs 180</t>
+  </si>
+  <si>
+    <t>halfcab to manual to bs flip</t>
+  </si>
+  <si>
+    <t>impossible</t>
+  </si>
+  <si>
+    <t>hydrant</t>
+  </si>
+  <si>
+    <t>fs 180 to fakie 5-0 to fakie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ollie to manual  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">360 flip  </t>
+  </si>
+  <si>
+    <t>switch fs 5050</t>
+  </si>
+  <si>
+    <t>bs smith to bs 180 to fakie manual to halfcab</t>
+  </si>
+  <si>
+    <t>ledge to manual</t>
+  </si>
+  <si>
+    <t>wallie to bs tailslide to fakie</t>
+  </si>
+  <si>
+    <t>wallie to ledge</t>
+  </si>
+  <si>
+    <t>switch fs tailslide to switch fs 5-0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bs flip to fakie manual to halfcab  </t>
+  </si>
+  <si>
+    <t>bs boardslide to bs feeble</t>
+  </si>
+  <si>
+    <t>switch fs feeble to regular</t>
+  </si>
+  <si>
+    <t>fs tailslide to kickflip to fakie</t>
+  </si>
+  <si>
+    <t>ledge to bank</t>
+  </si>
+  <si>
+    <t>bs feeble to wallride to fakie</t>
+  </si>
+  <si>
+    <t>ledge, wall</t>
+  </si>
+  <si>
+    <t>bs lipslide to wallride</t>
   </si>
 </sst>
 </file>
@@ -1378,11 +1654,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA88418-AAB9-4F27-A456-87056BC11CAB}">
-  <dimension ref="A1:J376"/>
+  <dimension ref="A1:J496"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I376" sqref="I376"/>
+      <pane ySplit="1" topLeftCell="A398" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N492" sqref="N492"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9351,6 +9627,2571 @@
         <v>298</v>
       </c>
     </row>
+    <row r="377" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A377">
+        <v>1</v>
+      </c>
+      <c r="B377">
+        <v>1</v>
+      </c>
+      <c r="C377" t="s">
+        <v>200</v>
+      </c>
+      <c r="G377" t="s">
+        <v>326</v>
+      </c>
+      <c r="J377" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="378" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A378">
+        <v>2</v>
+      </c>
+      <c r="B378">
+        <v>2</v>
+      </c>
+      <c r="C378" t="s">
+        <v>300</v>
+      </c>
+      <c r="G378" t="s">
+        <v>21</v>
+      </c>
+      <c r="H378" t="s">
+        <v>77</v>
+      </c>
+      <c r="J378" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="379" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A379">
+        <v>3</v>
+      </c>
+      <c r="B379">
+        <v>3</v>
+      </c>
+      <c r="C379" t="s">
+        <v>333</v>
+      </c>
+      <c r="G379" t="s">
+        <v>21</v>
+      </c>
+      <c r="H379" t="s">
+        <v>36</v>
+      </c>
+      <c r="J379" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="380" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A380">
+        <v>4</v>
+      </c>
+      <c r="B380">
+        <v>4</v>
+      </c>
+      <c r="C380" t="s">
+        <v>272</v>
+      </c>
+      <c r="G380" t="s">
+        <v>21</v>
+      </c>
+      <c r="H380" t="s">
+        <v>36</v>
+      </c>
+      <c r="J380" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="381" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A381">
+        <v>5</v>
+      </c>
+      <c r="B381">
+        <v>5</v>
+      </c>
+      <c r="C381" t="s">
+        <v>334</v>
+      </c>
+      <c r="D381">
+        <v>1</v>
+      </c>
+      <c r="G381" t="s">
+        <v>14</v>
+      </c>
+      <c r="H381" t="s">
+        <v>293</v>
+      </c>
+      <c r="J381" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="382" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A382">
+        <v>6</v>
+      </c>
+      <c r="B382">
+        <v>6</v>
+      </c>
+      <c r="C382" t="s">
+        <v>335</v>
+      </c>
+      <c r="G382" t="s">
+        <v>14</v>
+      </c>
+      <c r="H382" t="s">
+        <v>293</v>
+      </c>
+      <c r="J382" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="383" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A383">
+        <v>7</v>
+      </c>
+      <c r="B383">
+        <v>7</v>
+      </c>
+      <c r="C383" t="s">
+        <v>336</v>
+      </c>
+      <c r="G383" t="s">
+        <v>14</v>
+      </c>
+      <c r="H383" t="s">
+        <v>293</v>
+      </c>
+      <c r="J383" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="384" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A384">
+        <v>8</v>
+      </c>
+      <c r="B384">
+        <v>8</v>
+      </c>
+      <c r="C384" t="s">
+        <v>38</v>
+      </c>
+      <c r="E384">
+        <v>1</v>
+      </c>
+      <c r="G384" t="s">
+        <v>222</v>
+      </c>
+      <c r="J384" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="385" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A385">
+        <v>8</v>
+      </c>
+      <c r="B385">
+        <v>9</v>
+      </c>
+      <c r="C385" t="s">
+        <v>237</v>
+      </c>
+      <c r="E385">
+        <v>1</v>
+      </c>
+      <c r="G385" t="s">
+        <v>24</v>
+      </c>
+      <c r="H385" t="s">
+        <v>74</v>
+      </c>
+      <c r="J385" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="386" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A386">
+        <v>8</v>
+      </c>
+      <c r="B386">
+        <v>10</v>
+      </c>
+      <c r="C386" t="s">
+        <v>163</v>
+      </c>
+      <c r="E386">
+        <v>1</v>
+      </c>
+      <c r="G386" t="s">
+        <v>24</v>
+      </c>
+      <c r="J386" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="387" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A387">
+        <v>9</v>
+      </c>
+      <c r="B387">
+        <v>11</v>
+      </c>
+      <c r="C387" t="s">
+        <v>337</v>
+      </c>
+      <c r="D387">
+        <v>1</v>
+      </c>
+      <c r="G387" t="s">
+        <v>326</v>
+      </c>
+      <c r="J387" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="388" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A388">
+        <v>10</v>
+      </c>
+      <c r="B388">
+        <v>12</v>
+      </c>
+      <c r="C388" t="s">
+        <v>338</v>
+      </c>
+      <c r="E388">
+        <v>1</v>
+      </c>
+      <c r="G388" t="s">
+        <v>14</v>
+      </c>
+      <c r="J388" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="389" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A389">
+        <v>10</v>
+      </c>
+      <c r="B389">
+        <v>13</v>
+      </c>
+      <c r="C389" t="s">
+        <v>296</v>
+      </c>
+      <c r="E389">
+        <v>1</v>
+      </c>
+      <c r="G389" t="s">
+        <v>14</v>
+      </c>
+      <c r="J389" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="390" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A390">
+        <v>10</v>
+      </c>
+      <c r="B390">
+        <v>14</v>
+      </c>
+      <c r="C390" t="s">
+        <v>339</v>
+      </c>
+      <c r="E390">
+        <v>1</v>
+      </c>
+      <c r="G390" t="s">
+        <v>14</v>
+      </c>
+      <c r="J390" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="391" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A391">
+        <v>11</v>
+      </c>
+      <c r="B391">
+        <v>15</v>
+      </c>
+      <c r="C391" t="s">
+        <v>340</v>
+      </c>
+      <c r="G391" t="s">
+        <v>14</v>
+      </c>
+      <c r="H391" t="s">
+        <v>49</v>
+      </c>
+      <c r="J391" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="392" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A392">
+        <v>12</v>
+      </c>
+      <c r="B392">
+        <v>16</v>
+      </c>
+      <c r="C392" t="s">
+        <v>341</v>
+      </c>
+      <c r="D392">
+        <v>1</v>
+      </c>
+      <c r="G392" t="s">
+        <v>14</v>
+      </c>
+      <c r="H392" t="s">
+        <v>49</v>
+      </c>
+      <c r="J392" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="393" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A393">
+        <v>13</v>
+      </c>
+      <c r="B393">
+        <v>17</v>
+      </c>
+      <c r="C393" t="s">
+        <v>302</v>
+      </c>
+      <c r="D393">
+        <v>1</v>
+      </c>
+      <c r="G393" t="s">
+        <v>14</v>
+      </c>
+      <c r="J393" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="394" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A394">
+        <v>14</v>
+      </c>
+      <c r="B394">
+        <v>18</v>
+      </c>
+      <c r="C394" t="s">
+        <v>342</v>
+      </c>
+      <c r="F394">
+        <v>1</v>
+      </c>
+      <c r="G394" t="s">
+        <v>14</v>
+      </c>
+      <c r="H394" t="s">
+        <v>293</v>
+      </c>
+      <c r="J394" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="395" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A395">
+        <v>15</v>
+      </c>
+      <c r="B395">
+        <v>19</v>
+      </c>
+      <c r="C395" t="s">
+        <v>208</v>
+      </c>
+      <c r="D395">
+        <v>1</v>
+      </c>
+      <c r="F395">
+        <v>1</v>
+      </c>
+      <c r="G395" t="s">
+        <v>11</v>
+      </c>
+      <c r="J395" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="396" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A396">
+        <v>16</v>
+      </c>
+      <c r="B396">
+        <v>20</v>
+      </c>
+      <c r="C396" t="s">
+        <v>199</v>
+      </c>
+      <c r="D396">
+        <v>1</v>
+      </c>
+      <c r="F396">
+        <v>1</v>
+      </c>
+      <c r="G396" t="s">
+        <v>11</v>
+      </c>
+      <c r="J396" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="397" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A397">
+        <v>17</v>
+      </c>
+      <c r="B397">
+        <v>21</v>
+      </c>
+      <c r="C397" t="s">
+        <v>246</v>
+      </c>
+      <c r="D397">
+        <v>1</v>
+      </c>
+      <c r="F397">
+        <v>1</v>
+      </c>
+      <c r="G397" t="s">
+        <v>21</v>
+      </c>
+      <c r="H397" t="s">
+        <v>36</v>
+      </c>
+      <c r="J397" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="398" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A398">
+        <v>18</v>
+      </c>
+      <c r="B398">
+        <v>21</v>
+      </c>
+      <c r="C398" t="s">
+        <v>246</v>
+      </c>
+      <c r="D398">
+        <v>1</v>
+      </c>
+      <c r="F398">
+        <v>1</v>
+      </c>
+      <c r="G398" t="s">
+        <v>21</v>
+      </c>
+      <c r="H398" t="s">
+        <v>36</v>
+      </c>
+      <c r="J398" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="399" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A399">
+        <v>1</v>
+      </c>
+      <c r="B399">
+        <v>1</v>
+      </c>
+      <c r="C399" t="s">
+        <v>343</v>
+      </c>
+      <c r="E399">
+        <v>1</v>
+      </c>
+      <c r="G399" t="s">
+        <v>21</v>
+      </c>
+      <c r="H399" t="s">
+        <v>36</v>
+      </c>
+      <c r="J399" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="400" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A400">
+        <v>1</v>
+      </c>
+      <c r="B400">
+        <v>2</v>
+      </c>
+      <c r="C400" t="s">
+        <v>38</v>
+      </c>
+      <c r="E400">
+        <v>1</v>
+      </c>
+      <c r="G400" t="s">
+        <v>222</v>
+      </c>
+      <c r="J400" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="401" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A401">
+        <v>1</v>
+      </c>
+      <c r="B401">
+        <v>3</v>
+      </c>
+      <c r="C401" t="s">
+        <v>301</v>
+      </c>
+      <c r="E401">
+        <v>1</v>
+      </c>
+      <c r="G401" t="s">
+        <v>21</v>
+      </c>
+      <c r="H401" t="s">
+        <v>36</v>
+      </c>
+      <c r="J401" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="402" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A402">
+        <v>2</v>
+      </c>
+      <c r="B402">
+        <v>4</v>
+      </c>
+      <c r="C402" t="s">
+        <v>344</v>
+      </c>
+      <c r="G402" t="s">
+        <v>98</v>
+      </c>
+      <c r="H402" t="s">
+        <v>97</v>
+      </c>
+      <c r="J402" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="403" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A403">
+        <v>3</v>
+      </c>
+      <c r="B403">
+        <v>5</v>
+      </c>
+      <c r="C403" t="s">
+        <v>227</v>
+      </c>
+      <c r="D403">
+        <v>1</v>
+      </c>
+      <c r="G403" t="s">
+        <v>34</v>
+      </c>
+      <c r="J403" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="404" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A404">
+        <v>4</v>
+      </c>
+      <c r="B404">
+        <v>6</v>
+      </c>
+      <c r="C404" t="s">
+        <v>237</v>
+      </c>
+      <c r="G404" t="s">
+        <v>313</v>
+      </c>
+      <c r="J404" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="405" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A405">
+        <v>5</v>
+      </c>
+      <c r="B405">
+        <v>7</v>
+      </c>
+      <c r="C405" t="s">
+        <v>201</v>
+      </c>
+      <c r="G405" t="s">
+        <v>11</v>
+      </c>
+      <c r="H405" t="s">
+        <v>345</v>
+      </c>
+      <c r="J405" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="406" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A406">
+        <v>6</v>
+      </c>
+      <c r="B406">
+        <v>8</v>
+      </c>
+      <c r="C406" t="s">
+        <v>25</v>
+      </c>
+      <c r="G406" t="s">
+        <v>34</v>
+      </c>
+      <c r="H406" t="s">
+        <v>346</v>
+      </c>
+      <c r="J406" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="407" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A407">
+        <v>7</v>
+      </c>
+      <c r="B407">
+        <v>9</v>
+      </c>
+      <c r="C407" t="s">
+        <v>81</v>
+      </c>
+      <c r="G407" t="s">
+        <v>17</v>
+      </c>
+      <c r="J407" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="408" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A408">
+        <v>8</v>
+      </c>
+      <c r="B408">
+        <v>10</v>
+      </c>
+      <c r="C408" t="s">
+        <v>347</v>
+      </c>
+      <c r="G408" t="s">
+        <v>348</v>
+      </c>
+      <c r="J408" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="409" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A409">
+        <v>9</v>
+      </c>
+      <c r="B409">
+        <v>11</v>
+      </c>
+      <c r="C409" t="s">
+        <v>349</v>
+      </c>
+      <c r="G409" t="s">
+        <v>17</v>
+      </c>
+      <c r="J409" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="410" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A410">
+        <v>10</v>
+      </c>
+      <c r="B410">
+        <v>12</v>
+      </c>
+      <c r="C410" t="s">
+        <v>350</v>
+      </c>
+      <c r="G410" t="s">
+        <v>21</v>
+      </c>
+      <c r="H410" t="s">
+        <v>36</v>
+      </c>
+      <c r="J410" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="411" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A411">
+        <v>11</v>
+      </c>
+      <c r="B411">
+        <v>13</v>
+      </c>
+      <c r="C411" t="s">
+        <v>351</v>
+      </c>
+      <c r="G411" t="s">
+        <v>14</v>
+      </c>
+      <c r="J411" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="412" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A412">
+        <v>12</v>
+      </c>
+      <c r="B412">
+        <v>14</v>
+      </c>
+      <c r="C412" t="s">
+        <v>352</v>
+      </c>
+      <c r="D412">
+        <v>1</v>
+      </c>
+      <c r="G412" t="s">
+        <v>21</v>
+      </c>
+      <c r="H412" t="s">
+        <v>36</v>
+      </c>
+      <c r="J412" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="413" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A413">
+        <v>13</v>
+      </c>
+      <c r="B413">
+        <v>15</v>
+      </c>
+      <c r="C413" t="s">
+        <v>353</v>
+      </c>
+      <c r="D413">
+        <v>1</v>
+      </c>
+      <c r="G413" t="s">
+        <v>19</v>
+      </c>
+      <c r="H413" t="s">
+        <v>110</v>
+      </c>
+      <c r="J413" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="414" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A414">
+        <v>14</v>
+      </c>
+      <c r="B414">
+        <v>16</v>
+      </c>
+      <c r="C414" t="s">
+        <v>354</v>
+      </c>
+      <c r="D414">
+        <v>1</v>
+      </c>
+      <c r="E414">
+        <v>1</v>
+      </c>
+      <c r="G414" t="s">
+        <v>14</v>
+      </c>
+      <c r="J414" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="415" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A415">
+        <v>14</v>
+      </c>
+      <c r="B415">
+        <v>17</v>
+      </c>
+      <c r="C415" t="s">
+        <v>243</v>
+      </c>
+      <c r="D415">
+        <v>1</v>
+      </c>
+      <c r="E415">
+        <v>1</v>
+      </c>
+      <c r="G415" t="s">
+        <v>21</v>
+      </c>
+      <c r="H415" t="s">
+        <v>36</v>
+      </c>
+      <c r="J415" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="416" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A416">
+        <v>15</v>
+      </c>
+      <c r="B416">
+        <v>18</v>
+      </c>
+      <c r="C416" t="s">
+        <v>317</v>
+      </c>
+      <c r="E416">
+        <v>1</v>
+      </c>
+      <c r="G416" t="s">
+        <v>14</v>
+      </c>
+      <c r="J416" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="417" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A417">
+        <v>15</v>
+      </c>
+      <c r="B417">
+        <v>19</v>
+      </c>
+      <c r="C417" t="s">
+        <v>355</v>
+      </c>
+      <c r="E417">
+        <v>1</v>
+      </c>
+      <c r="G417" t="s">
+        <v>14</v>
+      </c>
+      <c r="J417" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="418" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A418">
+        <v>16</v>
+      </c>
+      <c r="B418">
+        <v>20</v>
+      </c>
+      <c r="C418" t="s">
+        <v>307</v>
+      </c>
+      <c r="F418">
+        <v>1</v>
+      </c>
+      <c r="G418" t="s">
+        <v>49</v>
+      </c>
+      <c r="J418" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="419" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A419">
+        <v>17</v>
+      </c>
+      <c r="B419">
+        <v>21</v>
+      </c>
+      <c r="C419" t="s">
+        <v>208</v>
+      </c>
+      <c r="D419">
+        <v>1</v>
+      </c>
+      <c r="E419">
+        <v>1</v>
+      </c>
+      <c r="G419" t="s">
+        <v>222</v>
+      </c>
+      <c r="J419" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="420" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A420">
+        <v>17</v>
+      </c>
+      <c r="B420">
+        <v>22</v>
+      </c>
+      <c r="C420" t="s">
+        <v>356</v>
+      </c>
+      <c r="E420">
+        <v>1</v>
+      </c>
+      <c r="G420" t="s">
+        <v>24</v>
+      </c>
+      <c r="J420" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="421" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A421">
+        <v>17</v>
+      </c>
+      <c r="B421">
+        <v>23</v>
+      </c>
+      <c r="C421" t="s">
+        <v>170</v>
+      </c>
+      <c r="D421">
+        <v>1</v>
+      </c>
+      <c r="E421">
+        <v>1</v>
+      </c>
+      <c r="G421" t="s">
+        <v>11</v>
+      </c>
+      <c r="J421" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="422" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A422">
+        <v>18</v>
+      </c>
+      <c r="B422">
+        <v>24</v>
+      </c>
+      <c r="C422" t="s">
+        <v>357</v>
+      </c>
+      <c r="E422">
+        <v>1</v>
+      </c>
+      <c r="G422" t="s">
+        <v>14</v>
+      </c>
+      <c r="J422" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="423" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A423">
+        <v>18</v>
+      </c>
+      <c r="B423">
+        <v>25</v>
+      </c>
+      <c r="C423" t="s">
+        <v>358</v>
+      </c>
+      <c r="D423">
+        <v>1</v>
+      </c>
+      <c r="E423">
+        <v>1</v>
+      </c>
+      <c r="G423" t="s">
+        <v>14</v>
+      </c>
+      <c r="J423" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="424" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A424">
+        <v>19</v>
+      </c>
+      <c r="B424">
+        <v>26</v>
+      </c>
+      <c r="C424" t="s">
+        <v>282</v>
+      </c>
+      <c r="D424">
+        <v>1</v>
+      </c>
+      <c r="E424">
+        <v>1</v>
+      </c>
+      <c r="G424" t="s">
+        <v>21</v>
+      </c>
+      <c r="H424" t="s">
+        <v>359</v>
+      </c>
+      <c r="J424" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="425" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A425">
+        <v>19</v>
+      </c>
+      <c r="B425">
+        <v>27</v>
+      </c>
+      <c r="C425" t="s">
+        <v>360</v>
+      </c>
+      <c r="E425">
+        <v>1</v>
+      </c>
+      <c r="G425" t="s">
+        <v>21</v>
+      </c>
+      <c r="H425" t="s">
+        <v>359</v>
+      </c>
+      <c r="J425" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="426" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A426">
+        <v>20</v>
+      </c>
+      <c r="B426">
+        <v>28</v>
+      </c>
+      <c r="C426" t="s">
+        <v>236</v>
+      </c>
+      <c r="E426">
+        <v>1</v>
+      </c>
+      <c r="G426" t="s">
+        <v>14</v>
+      </c>
+      <c r="J426" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="427" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A427">
+        <v>20</v>
+      </c>
+      <c r="B427">
+        <v>29</v>
+      </c>
+      <c r="C427" t="s">
+        <v>361</v>
+      </c>
+      <c r="D427">
+        <v>1</v>
+      </c>
+      <c r="E427">
+        <v>1</v>
+      </c>
+      <c r="G427" t="s">
+        <v>14</v>
+      </c>
+      <c r="J427" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="428" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A428">
+        <v>21</v>
+      </c>
+      <c r="B428">
+        <v>30</v>
+      </c>
+      <c r="C428" t="s">
+        <v>200</v>
+      </c>
+      <c r="E428">
+        <v>1</v>
+      </c>
+      <c r="G428" t="s">
+        <v>24</v>
+      </c>
+      <c r="H428" t="s">
+        <v>204</v>
+      </c>
+      <c r="J428" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="429" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A429">
+        <v>21</v>
+      </c>
+      <c r="B429">
+        <v>31</v>
+      </c>
+      <c r="C429" t="s">
+        <v>362</v>
+      </c>
+      <c r="E429">
+        <v>1</v>
+      </c>
+      <c r="G429" t="s">
+        <v>21</v>
+      </c>
+      <c r="H429" t="s">
+        <v>359</v>
+      </c>
+      <c r="J429" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="430" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A430">
+        <v>22</v>
+      </c>
+      <c r="B430">
+        <v>32</v>
+      </c>
+      <c r="C430" t="s">
+        <v>363</v>
+      </c>
+      <c r="G430" t="s">
+        <v>364</v>
+      </c>
+      <c r="J430" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="431" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A431">
+        <v>23</v>
+      </c>
+      <c r="B431">
+        <v>33</v>
+      </c>
+      <c r="C431" t="s">
+        <v>365</v>
+      </c>
+      <c r="D431">
+        <v>1</v>
+      </c>
+      <c r="G431" t="s">
+        <v>364</v>
+      </c>
+      <c r="J431" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="432" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A432">
+        <v>24</v>
+      </c>
+      <c r="B432">
+        <v>34</v>
+      </c>
+      <c r="C432" t="s">
+        <v>366</v>
+      </c>
+      <c r="G432" t="s">
+        <v>17</v>
+      </c>
+      <c r="J432" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="433" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A433">
+        <v>25</v>
+      </c>
+      <c r="B433">
+        <v>35</v>
+      </c>
+      <c r="C433" t="s">
+        <v>367</v>
+      </c>
+      <c r="D433">
+        <v>1</v>
+      </c>
+      <c r="G433" t="s">
+        <v>17</v>
+      </c>
+      <c r="J433" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="434" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A434">
+        <v>26</v>
+      </c>
+      <c r="B434">
+        <v>36</v>
+      </c>
+      <c r="C434" t="s">
+        <v>368</v>
+      </c>
+      <c r="D434">
+        <v>1</v>
+      </c>
+      <c r="G434" t="s">
+        <v>17</v>
+      </c>
+      <c r="H434" t="s">
+        <v>224</v>
+      </c>
+      <c r="J434" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="435" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A435">
+        <v>27</v>
+      </c>
+      <c r="B435">
+        <v>37</v>
+      </c>
+      <c r="C435" t="s">
+        <v>369</v>
+      </c>
+      <c r="G435" t="s">
+        <v>17</v>
+      </c>
+      <c r="J435" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="436" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A436">
+        <v>28</v>
+      </c>
+      <c r="B436">
+        <v>38</v>
+      </c>
+      <c r="C436" t="s">
+        <v>370</v>
+      </c>
+      <c r="G436" t="s">
+        <v>14</v>
+      </c>
+      <c r="H436" t="s">
+        <v>293</v>
+      </c>
+      <c r="J436" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="437" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A437">
+        <v>29</v>
+      </c>
+      <c r="B437">
+        <v>39</v>
+      </c>
+      <c r="C437" t="s">
+        <v>371</v>
+      </c>
+      <c r="F437">
+        <v>1</v>
+      </c>
+      <c r="G437" t="s">
+        <v>14</v>
+      </c>
+      <c r="J437" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="438" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A438">
+        <v>30</v>
+      </c>
+      <c r="B438">
+        <v>40</v>
+      </c>
+      <c r="C438" t="s">
+        <v>372</v>
+      </c>
+      <c r="G438" t="s">
+        <v>11</v>
+      </c>
+      <c r="J438" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="439" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A439">
+        <v>31</v>
+      </c>
+      <c r="B439">
+        <v>41</v>
+      </c>
+      <c r="C439" t="s">
+        <v>373</v>
+      </c>
+      <c r="G439" t="s">
+        <v>34</v>
+      </c>
+      <c r="H439" t="s">
+        <v>374</v>
+      </c>
+      <c r="J439" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="440" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A440">
+        <v>32</v>
+      </c>
+      <c r="B440">
+        <v>42</v>
+      </c>
+      <c r="C440" t="s">
+        <v>73</v>
+      </c>
+      <c r="D440">
+        <v>1</v>
+      </c>
+      <c r="G440" t="s">
+        <v>34</v>
+      </c>
+      <c r="H440" t="s">
+        <v>319</v>
+      </c>
+      <c r="J440" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="441" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A441">
+        <v>33</v>
+      </c>
+      <c r="B441">
+        <v>43</v>
+      </c>
+      <c r="C441" t="s">
+        <v>337</v>
+      </c>
+      <c r="D441">
+        <v>1</v>
+      </c>
+      <c r="G441" t="s">
+        <v>34</v>
+      </c>
+      <c r="H441" t="s">
+        <v>319</v>
+      </c>
+      <c r="J441" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="442" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A442">
+        <v>34</v>
+      </c>
+      <c r="B442">
+        <v>44</v>
+      </c>
+      <c r="C442" t="s">
+        <v>375</v>
+      </c>
+      <c r="D442">
+        <v>1</v>
+      </c>
+      <c r="G442" t="s">
+        <v>11</v>
+      </c>
+      <c r="H442" t="s">
+        <v>376</v>
+      </c>
+      <c r="J442" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="443" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A443">
+        <v>35</v>
+      </c>
+      <c r="B443">
+        <v>45</v>
+      </c>
+      <c r="C443" t="s">
+        <v>62</v>
+      </c>
+      <c r="D443">
+        <v>1</v>
+      </c>
+      <c r="G443" t="s">
+        <v>377</v>
+      </c>
+      <c r="H443" t="s">
+        <v>376</v>
+      </c>
+      <c r="J443" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="444" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A444">
+        <v>36</v>
+      </c>
+      <c r="B444">
+        <v>45</v>
+      </c>
+      <c r="C444" t="s">
+        <v>62</v>
+      </c>
+      <c r="D444">
+        <v>1</v>
+      </c>
+      <c r="G444" t="s">
+        <v>11</v>
+      </c>
+      <c r="H444" t="s">
+        <v>376</v>
+      </c>
+      <c r="J444" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="445" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A445">
+        <v>37</v>
+      </c>
+      <c r="B445">
+        <v>46</v>
+      </c>
+      <c r="C445" t="s">
+        <v>378</v>
+      </c>
+      <c r="G445" t="s">
+        <v>14</v>
+      </c>
+      <c r="J445" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="446" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A446">
+        <v>38</v>
+      </c>
+      <c r="B446">
+        <v>47</v>
+      </c>
+      <c r="C446" t="s">
+        <v>29</v>
+      </c>
+      <c r="D446">
+        <v>1</v>
+      </c>
+      <c r="F446">
+        <v>1</v>
+      </c>
+      <c r="G446" t="s">
+        <v>11</v>
+      </c>
+      <c r="H446" t="s">
+        <v>379</v>
+      </c>
+      <c r="J446" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="447" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A447">
+        <v>39</v>
+      </c>
+      <c r="B447">
+        <v>47</v>
+      </c>
+      <c r="C447" t="s">
+        <v>29</v>
+      </c>
+      <c r="D447">
+        <v>1</v>
+      </c>
+      <c r="F447">
+        <v>1</v>
+      </c>
+      <c r="G447" t="s">
+        <v>11</v>
+      </c>
+      <c r="H447" t="s">
+        <v>379</v>
+      </c>
+      <c r="J447" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="448" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A448">
+        <v>40</v>
+      </c>
+      <c r="B448">
+        <v>48</v>
+      </c>
+      <c r="C448" t="s">
+        <v>380</v>
+      </c>
+      <c r="D448">
+        <v>1</v>
+      </c>
+      <c r="F448">
+        <v>1</v>
+      </c>
+      <c r="G448" t="s">
+        <v>11</v>
+      </c>
+      <c r="H448" t="s">
+        <v>379</v>
+      </c>
+      <c r="J448" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="449" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A449">
+        <v>41</v>
+      </c>
+      <c r="B449">
+        <v>49</v>
+      </c>
+      <c r="C449" t="s">
+        <v>195</v>
+      </c>
+      <c r="D449">
+        <v>1</v>
+      </c>
+      <c r="G449" t="s">
+        <v>11</v>
+      </c>
+      <c r="J449" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="450" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A450">
+        <v>42</v>
+      </c>
+      <c r="B450">
+        <v>50</v>
+      </c>
+      <c r="C450" t="s">
+        <v>381</v>
+      </c>
+      <c r="D450">
+        <v>1</v>
+      </c>
+      <c r="F450">
+        <v>1</v>
+      </c>
+      <c r="G450" t="s">
+        <v>21</v>
+      </c>
+      <c r="H450" t="s">
+        <v>36</v>
+      </c>
+      <c r="J450" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="451" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A451">
+        <v>43</v>
+      </c>
+      <c r="B451">
+        <v>50</v>
+      </c>
+      <c r="C451" t="s">
+        <v>381</v>
+      </c>
+      <c r="D451">
+        <v>1</v>
+      </c>
+      <c r="F451">
+        <v>1</v>
+      </c>
+      <c r="G451" t="s">
+        <v>21</v>
+      </c>
+      <c r="H451" t="s">
+        <v>36</v>
+      </c>
+      <c r="J451" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="452" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A452">
+        <v>44</v>
+      </c>
+      <c r="B452">
+        <v>51</v>
+      </c>
+      <c r="C452" t="s">
+        <v>282</v>
+      </c>
+      <c r="D452">
+        <v>1</v>
+      </c>
+      <c r="F452">
+        <v>1</v>
+      </c>
+      <c r="G452" t="s">
+        <v>21</v>
+      </c>
+      <c r="H452" t="s">
+        <v>36</v>
+      </c>
+      <c r="J452" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="453" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A453">
+        <v>45</v>
+      </c>
+      <c r="B453">
+        <v>52</v>
+      </c>
+      <c r="C453" t="s">
+        <v>382</v>
+      </c>
+      <c r="D453">
+        <v>1</v>
+      </c>
+      <c r="F453">
+        <v>1</v>
+      </c>
+      <c r="G453" t="s">
+        <v>21</v>
+      </c>
+      <c r="H453" t="s">
+        <v>36</v>
+      </c>
+      <c r="J453" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="454" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A454">
+        <v>46</v>
+      </c>
+      <c r="B454">
+        <v>52</v>
+      </c>
+      <c r="C454" t="s">
+        <v>382</v>
+      </c>
+      <c r="D454">
+        <v>1</v>
+      </c>
+      <c r="F454">
+        <v>1</v>
+      </c>
+      <c r="G454" t="s">
+        <v>21</v>
+      </c>
+      <c r="H454" t="s">
+        <v>36</v>
+      </c>
+      <c r="J454" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="455" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A455">
+        <v>47</v>
+      </c>
+      <c r="B455">
+        <v>53</v>
+      </c>
+      <c r="C455" t="s">
+        <v>383</v>
+      </c>
+      <c r="F455">
+        <v>1</v>
+      </c>
+      <c r="G455" t="s">
+        <v>11</v>
+      </c>
+      <c r="H455" t="s">
+        <v>384</v>
+      </c>
+      <c r="J455" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="456" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A456">
+        <v>48</v>
+      </c>
+      <c r="B456">
+        <v>53</v>
+      </c>
+      <c r="C456" t="s">
+        <v>383</v>
+      </c>
+      <c r="F456">
+        <v>1</v>
+      </c>
+      <c r="G456" t="s">
+        <v>11</v>
+      </c>
+      <c r="H456" t="s">
+        <v>384</v>
+      </c>
+      <c r="J456" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="457" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A457">
+        <v>1</v>
+      </c>
+      <c r="B457">
+        <v>1</v>
+      </c>
+      <c r="C457" t="s">
+        <v>264</v>
+      </c>
+      <c r="G457" t="s">
+        <v>21</v>
+      </c>
+      <c r="H457" t="s">
+        <v>77</v>
+      </c>
+      <c r="J457" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="458" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A458">
+        <v>2</v>
+      </c>
+      <c r="B458">
+        <v>2</v>
+      </c>
+      <c r="C458" t="s">
+        <v>387</v>
+      </c>
+      <c r="G458" t="s">
+        <v>265</v>
+      </c>
+      <c r="H458" t="s">
+        <v>391</v>
+      </c>
+      <c r="J458" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="459" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A459">
+        <v>3</v>
+      </c>
+      <c r="B459">
+        <v>3</v>
+      </c>
+      <c r="C459" t="s">
+        <v>388</v>
+      </c>
+      <c r="E459">
+        <v>1</v>
+      </c>
+      <c r="G459" t="s">
+        <v>17</v>
+      </c>
+      <c r="J459" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="460" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A460">
+        <v>3</v>
+      </c>
+      <c r="B460">
+        <v>4</v>
+      </c>
+      <c r="C460" t="s">
+        <v>389</v>
+      </c>
+      <c r="E460">
+        <v>1</v>
+      </c>
+      <c r="G460" t="s">
+        <v>390</v>
+      </c>
+      <c r="H460" t="s">
+        <v>391</v>
+      </c>
+      <c r="J460" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="461" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A461">
+        <v>4</v>
+      </c>
+      <c r="B461">
+        <v>5</v>
+      </c>
+      <c r="C461" t="s">
+        <v>392</v>
+      </c>
+      <c r="G461" t="s">
+        <v>14</v>
+      </c>
+      <c r="J461" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="462" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A462">
+        <v>5</v>
+      </c>
+      <c r="B462">
+        <v>6</v>
+      </c>
+      <c r="C462" t="s">
+        <v>393</v>
+      </c>
+      <c r="G462" t="s">
+        <v>394</v>
+      </c>
+      <c r="H462" t="s">
+        <v>399</v>
+      </c>
+      <c r="J462" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="463" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A463">
+        <v>6</v>
+      </c>
+      <c r="B463">
+        <v>7</v>
+      </c>
+      <c r="C463" t="s">
+        <v>395</v>
+      </c>
+      <c r="G463" t="s">
+        <v>14</v>
+      </c>
+      <c r="J463" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="464" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A464">
+        <v>7</v>
+      </c>
+      <c r="B464">
+        <v>7</v>
+      </c>
+      <c r="C464" t="s">
+        <v>395</v>
+      </c>
+      <c r="G464" t="s">
+        <v>14</v>
+      </c>
+      <c r="J464" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="465" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A465">
+        <v>8</v>
+      </c>
+      <c r="B465">
+        <v>8</v>
+      </c>
+      <c r="C465" t="s">
+        <v>396</v>
+      </c>
+      <c r="G465" t="s">
+        <v>14</v>
+      </c>
+      <c r="H465" t="s">
+        <v>397</v>
+      </c>
+      <c r="J465" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="466" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A466">
+        <v>9</v>
+      </c>
+      <c r="B466">
+        <v>9</v>
+      </c>
+      <c r="C466" t="s">
+        <v>398</v>
+      </c>
+      <c r="G466" t="s">
+        <v>394</v>
+      </c>
+      <c r="H466" t="s">
+        <v>391</v>
+      </c>
+      <c r="J466" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="467" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A467">
+        <v>10</v>
+      </c>
+      <c r="B467">
+        <v>10</v>
+      </c>
+      <c r="C467" t="s">
+        <v>400</v>
+      </c>
+      <c r="G467" t="s">
+        <v>14</v>
+      </c>
+      <c r="H467" t="s">
+        <v>401</v>
+      </c>
+      <c r="J467" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="468" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A468">
+        <v>11</v>
+      </c>
+      <c r="B468">
+        <v>11</v>
+      </c>
+      <c r="C468" t="s">
+        <v>25</v>
+      </c>
+      <c r="G468" t="s">
+        <v>402</v>
+      </c>
+      <c r="H468" t="s">
+        <v>204</v>
+      </c>
+      <c r="J468" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="469" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A469">
+        <v>12</v>
+      </c>
+      <c r="B469">
+        <v>12</v>
+      </c>
+      <c r="C469" t="s">
+        <v>25</v>
+      </c>
+      <c r="F469">
+        <v>1</v>
+      </c>
+      <c r="G469" t="s">
+        <v>402</v>
+      </c>
+      <c r="H469" t="s">
+        <v>204</v>
+      </c>
+      <c r="J469" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="470" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A470">
+        <v>13</v>
+      </c>
+      <c r="B470">
+        <v>13</v>
+      </c>
+      <c r="C470" t="s">
+        <v>403</v>
+      </c>
+      <c r="E470">
+        <v>1</v>
+      </c>
+      <c r="G470" t="s">
+        <v>389</v>
+      </c>
+      <c r="H470" t="s">
+        <v>391</v>
+      </c>
+      <c r="J470" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="471" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A471">
+        <v>13</v>
+      </c>
+      <c r="B471">
+        <v>14</v>
+      </c>
+      <c r="C471" t="s">
+        <v>404</v>
+      </c>
+      <c r="E471">
+        <v>1</v>
+      </c>
+      <c r="G471" t="s">
+        <v>17</v>
+      </c>
+      <c r="J471" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="472" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A472">
+        <v>14</v>
+      </c>
+      <c r="B472">
+        <v>15</v>
+      </c>
+      <c r="C472" t="s">
+        <v>393</v>
+      </c>
+      <c r="E472">
+        <v>1</v>
+      </c>
+      <c r="G472" t="s">
+        <v>394</v>
+      </c>
+      <c r="H472" t="s">
+        <v>391</v>
+      </c>
+      <c r="J472" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="473" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A473">
+        <v>15</v>
+      </c>
+      <c r="B473">
+        <v>16</v>
+      </c>
+      <c r="C473" t="s">
+        <v>405</v>
+      </c>
+      <c r="E473">
+        <v>1</v>
+      </c>
+      <c r="F473">
+        <v>1</v>
+      </c>
+      <c r="G473" t="s">
+        <v>406</v>
+      </c>
+      <c r="H473" t="s">
+        <v>204</v>
+      </c>
+      <c r="J473" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="474" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A474">
+        <v>16</v>
+      </c>
+      <c r="B474">
+        <v>17</v>
+      </c>
+      <c r="C474" t="s">
+        <v>407</v>
+      </c>
+      <c r="G474" t="s">
+        <v>21</v>
+      </c>
+      <c r="H474" t="s">
+        <v>93</v>
+      </c>
+      <c r="J474" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="475" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A475">
+        <v>17</v>
+      </c>
+      <c r="B475">
+        <v>18</v>
+      </c>
+      <c r="C475" t="s">
+        <v>336</v>
+      </c>
+      <c r="F475">
+        <v>1</v>
+      </c>
+      <c r="G475" t="s">
+        <v>21</v>
+      </c>
+      <c r="H475" t="s">
+        <v>93</v>
+      </c>
+      <c r="J475" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="476" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A476">
+        <v>18</v>
+      </c>
+      <c r="B476">
+        <v>19</v>
+      </c>
+      <c r="C476" t="s">
+        <v>408</v>
+      </c>
+      <c r="E476">
+        <v>1</v>
+      </c>
+      <c r="G476" t="s">
+        <v>17</v>
+      </c>
+      <c r="H476" t="s">
+        <v>137</v>
+      </c>
+      <c r="J476" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="477" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A477">
+        <v>18</v>
+      </c>
+      <c r="B477">
+        <v>20</v>
+      </c>
+      <c r="C477" t="s">
+        <v>409</v>
+      </c>
+      <c r="E477">
+        <v>1</v>
+      </c>
+      <c r="G477" t="s">
+        <v>215</v>
+      </c>
+      <c r="H477" t="s">
+        <v>204</v>
+      </c>
+      <c r="J477" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="478" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A478">
+        <v>19</v>
+      </c>
+      <c r="B478">
+        <v>21</v>
+      </c>
+      <c r="C478" t="s">
+        <v>373</v>
+      </c>
+      <c r="G478" t="s">
+        <v>215</v>
+      </c>
+      <c r="H478" t="s">
+        <v>204</v>
+      </c>
+      <c r="J478" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="479" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A479">
+        <v>20</v>
+      </c>
+      <c r="B479">
+        <v>22</v>
+      </c>
+      <c r="C479" t="s">
+        <v>410</v>
+      </c>
+      <c r="D479">
+        <v>1</v>
+      </c>
+      <c r="G479" t="s">
+        <v>21</v>
+      </c>
+      <c r="H479" t="s">
+        <v>36</v>
+      </c>
+      <c r="J479" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="480" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A480">
+        <v>21</v>
+      </c>
+      <c r="B480">
+        <v>23</v>
+      </c>
+      <c r="C480" t="s">
+        <v>411</v>
+      </c>
+      <c r="G480" t="s">
+        <v>412</v>
+      </c>
+      <c r="H480" t="s">
+        <v>17</v>
+      </c>
+      <c r="J480" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="481" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A481">
+        <v>22</v>
+      </c>
+      <c r="B481">
+        <v>24</v>
+      </c>
+      <c r="C481" t="s">
+        <v>368</v>
+      </c>
+      <c r="D481">
+        <v>1</v>
+      </c>
+      <c r="G481" t="s">
+        <v>17</v>
+      </c>
+      <c r="H481" t="s">
+        <v>224</v>
+      </c>
+      <c r="J481" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="482" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A482">
+        <v>23</v>
+      </c>
+      <c r="B482">
+        <v>25</v>
+      </c>
+      <c r="C482" t="s">
+        <v>413</v>
+      </c>
+      <c r="F482">
+        <v>1</v>
+      </c>
+      <c r="G482" t="s">
+        <v>414</v>
+      </c>
+      <c r="J482" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="483" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A483">
+        <v>24</v>
+      </c>
+      <c r="B483">
+        <v>25</v>
+      </c>
+      <c r="C483" t="s">
+        <v>413</v>
+      </c>
+      <c r="G483" t="s">
+        <v>414</v>
+      </c>
+      <c r="J483" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="484" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A484">
+        <v>25</v>
+      </c>
+      <c r="B484">
+        <v>26</v>
+      </c>
+      <c r="C484" t="s">
+        <v>415</v>
+      </c>
+      <c r="D484">
+        <v>1</v>
+      </c>
+      <c r="G484" t="s">
+        <v>14</v>
+      </c>
+      <c r="J484" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="485" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A485">
+        <v>26</v>
+      </c>
+      <c r="B485">
+        <v>27</v>
+      </c>
+      <c r="C485" t="s">
+        <v>416</v>
+      </c>
+      <c r="G485" t="s">
+        <v>17</v>
+      </c>
+      <c r="J485" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="486" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A486">
+        <v>27</v>
+      </c>
+      <c r="B486">
+        <v>28</v>
+      </c>
+      <c r="C486" t="s">
+        <v>417</v>
+      </c>
+      <c r="F486">
+        <v>1</v>
+      </c>
+      <c r="G486" t="s">
+        <v>21</v>
+      </c>
+      <c r="H486" t="s">
+        <v>36</v>
+      </c>
+      <c r="J486" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="487" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A487">
+        <v>28</v>
+      </c>
+      <c r="B487">
+        <v>28</v>
+      </c>
+      <c r="C487" t="s">
+        <v>417</v>
+      </c>
+      <c r="G487" t="s">
+        <v>21</v>
+      </c>
+      <c r="H487" t="s">
+        <v>36</v>
+      </c>
+      <c r="J487" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="488" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A488">
+        <v>29</v>
+      </c>
+      <c r="B488">
+        <v>29</v>
+      </c>
+      <c r="C488" t="s">
+        <v>418</v>
+      </c>
+      <c r="D488">
+        <v>1</v>
+      </c>
+      <c r="G488" t="s">
+        <v>98</v>
+      </c>
+      <c r="H488" t="s">
+        <v>265</v>
+      </c>
+      <c r="J488" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="489" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A489">
+        <v>30</v>
+      </c>
+      <c r="B489">
+        <v>29</v>
+      </c>
+      <c r="C489" t="s">
+        <v>418</v>
+      </c>
+      <c r="D489">
+        <v>1</v>
+      </c>
+      <c r="E489">
+        <v>1</v>
+      </c>
+      <c r="G489" t="s">
+        <v>98</v>
+      </c>
+      <c r="H489" t="s">
+        <v>265</v>
+      </c>
+      <c r="J489" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="490" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A490">
+        <v>30</v>
+      </c>
+      <c r="B490">
+        <v>30</v>
+      </c>
+      <c r="C490" t="s">
+        <v>65</v>
+      </c>
+      <c r="D490">
+        <v>1</v>
+      </c>
+      <c r="E490">
+        <v>1</v>
+      </c>
+      <c r="G490" t="s">
+        <v>24</v>
+      </c>
+      <c r="J490" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="491" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A491">
+        <v>31</v>
+      </c>
+      <c r="B491">
+        <v>31</v>
+      </c>
+      <c r="C491" t="s">
+        <v>419</v>
+      </c>
+      <c r="F491">
+        <v>1</v>
+      </c>
+      <c r="G491" t="s">
+        <v>14</v>
+      </c>
+      <c r="H491" t="s">
+        <v>420</v>
+      </c>
+      <c r="J491" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="492" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A492">
+        <v>32</v>
+      </c>
+      <c r="B492">
+        <v>32</v>
+      </c>
+      <c r="C492" t="s">
+        <v>407</v>
+      </c>
+      <c r="F492">
+        <v>1</v>
+      </c>
+      <c r="G492" t="s">
+        <v>98</v>
+      </c>
+      <c r="H492" t="s">
+        <v>265</v>
+      </c>
+      <c r="J492" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="493" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A493">
+        <v>33</v>
+      </c>
+      <c r="B493">
+        <v>32</v>
+      </c>
+      <c r="C493" t="s">
+        <v>407</v>
+      </c>
+      <c r="G493" t="s">
+        <v>98</v>
+      </c>
+      <c r="H493" t="s">
+        <v>265</v>
+      </c>
+      <c r="J493" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="494" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A494">
+        <v>34</v>
+      </c>
+      <c r="B494">
+        <v>33</v>
+      </c>
+      <c r="C494" t="s">
+        <v>421</v>
+      </c>
+      <c r="F494">
+        <v>1</v>
+      </c>
+      <c r="G494" t="s">
+        <v>401</v>
+      </c>
+      <c r="H494" t="s">
+        <v>422</v>
+      </c>
+      <c r="J494" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="495" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A495">
+        <v>35</v>
+      </c>
+      <c r="B495">
+        <v>34</v>
+      </c>
+      <c r="C495" t="s">
+        <v>423</v>
+      </c>
+      <c r="F495">
+        <v>1</v>
+      </c>
+      <c r="G495" t="s">
+        <v>401</v>
+      </c>
+      <c r="H495" t="s">
+        <v>422</v>
+      </c>
+      <c r="J495" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="496" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A496">
+        <v>36</v>
+      </c>
+      <c r="B496">
+        <v>34</v>
+      </c>
+      <c r="C496" t="s">
+        <v>423</v>
+      </c>
+      <c r="F496">
+        <v>1</v>
+      </c>
+      <c r="G496" t="s">
+        <v>401</v>
+      </c>
+      <c r="H496" t="s">
+        <v>422</v>
+      </c>
+      <c r="J496" t="s">
+        <v>386</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>